<commit_message>
Plan de Estimación e Iteración
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/01-Inicio/05- Gestion de Proyecto/TP052-OO-PCU y PCU Ajustados_Testify V2.xlsx
+++ b/Fases_de_desarrollo/01-Inicio/05- Gestion de Proyecto/TP052-OO-PCU y PCU Ajustados_Testify V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valeria\Documents\Oslo\Testify\Testify\Fases_de_desarrollo\01-Inicio\05- Gestion de Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veo_2\OneDrive\Documentos\Testify\Fases_de_desarrollo\01-Inicio\05- Gestion de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11436"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecto1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
   <authors>
     <author>Leonardo G A</author>
     <author>Leonardo Gonzalez</author>
+    <author>Valeria Ojeda Muñoz</author>
   </authors>
   <commentList>
     <comment ref="C7" authorId="0" shapeId="0">
@@ -105,6 +106,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="D80" authorId="2" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valeria Ojeda Muñoz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Modificado</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -479,7 +504,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -555,6 +580,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1319,25 +1357,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:T104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81:D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="32.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
+    <col min="10" max="10" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" s="53" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:20" s="53" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="52" t="s">
         <v>58</v>
       </c>
@@ -1347,7 +1385,7 @@
       <c r="G2" s="52"/>
       <c r="H2" s="52"/>
     </row>
-    <row r="3" spans="2:20" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" s="53" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="51" t="s">
         <v>88</v>
       </c>
@@ -1357,7 +1395,7 @@
       <c r="G3" s="54"/>
       <c r="H3" s="54"/>
     </row>
-    <row r="4" spans="2:20" s="53" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:20" s="53" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="51"/>
       <c r="D4" s="54"/>
       <c r="E4" s="54"/>
@@ -1365,7 +1403,7 @@
       <c r="G4" s="54"/>
       <c r="H4" s="54"/>
     </row>
-    <row r="5" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="29"/>
       <c r="C5" s="1"/>
       <c r="D5" s="20"/>
@@ -1374,7 +1412,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
-    <row r="7" spans="2:20" s="9" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:20" s="9" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
@@ -1395,7 +1433,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>69</v>
       </c>
@@ -1418,7 +1456,7 @@
       </c>
       <c r="H8" s="27"/>
     </row>
-    <row r="9" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>70</v>
       </c>
@@ -1441,7 +1479,7 @@
       </c>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>71</v>
       </c>
@@ -1464,7 +1502,7 @@
       </c>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="2:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:20" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>72</v>
       </c>
@@ -1487,7 +1525,7 @@
       </c>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="2:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:20" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>73</v>
       </c>
@@ -1510,7 +1548,7 @@
       </c>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="2:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:20" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13"/>
       <c r="C13" s="89" t="s">
         <v>53</v>
@@ -1524,7 +1562,7 @@
       </c>
       <c r="H13" s="17"/>
     </row>
-    <row r="14" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
@@ -1533,7 +1571,7 @@
       <c r="G14" s="34"/>
       <c r="H14" s="17"/>
     </row>
-    <row r="15" spans="2:20" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:20" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1542,7 +1580,7 @@
       <c r="G15" s="18"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="2:20" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:20" s="19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>36</v>
       </c>
@@ -1562,7 +1600,7 @@
       <c r="H16" s="21"/>
       <c r="T16" s="22"/>
     </row>
-    <row r="17" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>118</v>
       </c>
@@ -1583,7 +1621,7 @@
       <c r="K17" s="22"/>
       <c r="T17" s="22"/>
     </row>
-    <row r="18" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>89</v>
       </c>
@@ -1604,7 +1642,7 @@
       <c r="K18" s="22"/>
       <c r="T18" s="22"/>
     </row>
-    <row r="19" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>90</v>
       </c>
@@ -1625,7 +1663,7 @@
       <c r="K19" s="22"/>
       <c r="T19" s="22"/>
     </row>
-    <row r="20" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>91</v>
       </c>
@@ -1646,7 +1684,7 @@
       <c r="K20" s="22"/>
       <c r="T20" s="22"/>
     </row>
-    <row r="21" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>119</v>
       </c>
@@ -1667,7 +1705,7 @@
       <c r="K21" s="22"/>
       <c r="T21" s="22"/>
     </row>
-    <row r="22" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
         <v>96</v>
       </c>
@@ -1688,7 +1726,7 @@
       <c r="K22" s="22"/>
       <c r="T22" s="22"/>
     </row>
-    <row r="23" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>92</v>
       </c>
@@ -1709,7 +1747,7 @@
       <c r="K23" s="22"/>
       <c r="T23" s="22"/>
     </row>
-    <row r="24" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
         <v>97</v>
       </c>
@@ -1730,7 +1768,7 @@
       <c r="K24" s="22"/>
       <c r="T24" s="22"/>
     </row>
-    <row r="25" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>93</v>
       </c>
@@ -1751,7 +1789,7 @@
       <c r="K25" s="22"/>
       <c r="T25" s="22"/>
     </row>
-    <row r="26" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10" t="s">
         <v>94</v>
       </c>
@@ -1772,7 +1810,7 @@
       <c r="K26" s="22"/>
       <c r="T26" s="22"/>
     </row>
-    <row r="27" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>98</v>
       </c>
@@ -1793,7 +1831,7 @@
       <c r="K27" s="22"/>
       <c r="T27" s="22"/>
     </row>
-    <row r="28" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
         <v>95</v>
       </c>
@@ -1814,7 +1852,7 @@
       <c r="K28" s="22"/>
       <c r="T28" s="22"/>
     </row>
-    <row r="29" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>99</v>
       </c>
@@ -1835,7 +1873,7 @@
       <c r="K29" s="22"/>
       <c r="T29" s="22"/>
     </row>
-    <row r="30" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
         <v>100</v>
       </c>
@@ -1856,7 +1894,7 @@
       <c r="K30" s="22"/>
       <c r="T30" s="22"/>
     </row>
-    <row r="31" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>101</v>
       </c>
@@ -1877,7 +1915,7 @@
       <c r="K31" s="22"/>
       <c r="T31" s="22"/>
     </row>
-    <row r="32" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>102</v>
       </c>
@@ -1898,7 +1936,7 @@
       <c r="K32" s="22"/>
       <c r="T32" s="22"/>
     </row>
-    <row r="33" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
         <v>103</v>
       </c>
@@ -1919,7 +1957,7 @@
       <c r="K33" s="22"/>
       <c r="T33" s="22"/>
     </row>
-    <row r="34" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>104</v>
       </c>
@@ -1940,7 +1978,7 @@
       <c r="K34" s="22"/>
       <c r="T34" s="22"/>
     </row>
-    <row r="35" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="10" t="s">
         <v>105</v>
       </c>
@@ -1961,7 +1999,7 @@
       <c r="K35" s="22"/>
       <c r="T35" s="22"/>
     </row>
-    <row r="36" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>106</v>
       </c>
@@ -1982,7 +2020,7 @@
       <c r="K36" s="22"/>
       <c r="T36" s="22"/>
     </row>
-    <row r="37" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>107</v>
       </c>
@@ -2003,7 +2041,7 @@
       <c r="K37" s="22"/>
       <c r="T37" s="22"/>
     </row>
-    <row r="38" spans="2:20" s="19" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:20" s="19" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="44"/>
       <c r="C38" s="91" t="s">
         <v>54</v>
@@ -2017,13 +2055,13 @@
       <c r="H38" s="17"/>
       <c r="K38" s="22"/>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H40" s="27"/>
     </row>
-    <row r="41" spans="2:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:20" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13"/>
       <c r="C41" s="89" t="s">
         <v>55</v>
@@ -2036,9 +2074,9 @@
       </c>
       <c r="H41" s="17"/>
     </row>
-    <row r="42" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="2:20" s="9" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:20" s="9" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="35" t="s">
         <v>6</v>
       </c>
@@ -2058,7 +2096,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:20" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="24" t="s">
         <v>8</v>
       </c>
@@ -2080,7 +2118,7 @@
       </c>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="24" t="s">
         <v>9</v>
       </c>
@@ -2102,7 +2140,7 @@
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="24" t="s">
         <v>10</v>
       </c>
@@ -2124,7 +2162,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:20" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="24" t="s">
         <v>11</v>
       </c>
@@ -2144,7 +2182,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="24" t="s">
         <v>12</v>
       </c>
@@ -2166,7 +2204,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="24" t="s">
         <v>13</v>
       </c>
@@ -2188,7 +2226,7 @@
       </c>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="24" t="s">
         <v>14</v>
       </c>
@@ -2210,7 +2248,7 @@
       </c>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="24" t="s">
         <v>15</v>
       </c>
@@ -2232,7 +2270,7 @@
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="24" t="s">
         <v>16</v>
       </c>
@@ -2252,7 +2290,7 @@
       </c>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="24" t="s">
         <v>17</v>
       </c>
@@ -2272,7 +2310,7 @@
       </c>
       <c r="H54" s="1"/>
     </row>
-    <row r="55" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="24" t="s">
         <v>18</v>
       </c>
@@ -2294,7 +2332,7 @@
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="24" t="s">
         <v>19</v>
       </c>
@@ -2316,7 +2354,7 @@
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" spans="2:8" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="24" t="s">
         <v>20</v>
       </c>
@@ -2338,7 +2376,7 @@
       </c>
       <c r="H57" s="1"/>
     </row>
-    <row r="58" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="84" t="s">
         <v>21</v>
       </c>
@@ -2352,7 +2390,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="84" t="s">
         <v>39</v>
       </c>
@@ -2366,7 +2404,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="31"/>
       <c r="C60" s="55"/>
       <c r="D60" s="55"/>
@@ -2374,7 +2412,7 @@
       <c r="F60" s="55"/>
       <c r="H60" s="1"/>
     </row>
-    <row r="61" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="46"/>
       <c r="C61" s="47"/>
       <c r="D61" s="48"/>
@@ -2382,7 +2420,7 @@
       <c r="F61" s="49"/>
       <c r="G61" s="46"/>
     </row>
-    <row r="62" spans="2:8" s="9" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:8" s="9" customFormat="1" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="35" t="s">
         <v>23</v>
       </c>
@@ -2402,7 +2440,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="25" t="s">
         <v>44</v>
       </c>
@@ -2423,7 +2461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:8" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="25" t="s">
         <v>45</v>
       </c>
@@ -2444,7 +2482,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="25" t="s">
         <v>46</v>
       </c>
@@ -2465,7 +2503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="25" t="s">
         <v>47</v>
       </c>
@@ -2486,7 +2524,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="25" t="s">
         <v>48</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="25" t="s">
         <v>49</v>
       </c>
@@ -2528,7 +2566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="63" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:7" ht="62.4" x14ac:dyDescent="0.25">
       <c r="B69" s="25" t="s">
         <v>50</v>
       </c>
@@ -2549,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="110.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" ht="109.2" x14ac:dyDescent="0.25">
       <c r="B70" s="25" t="s">
         <v>52</v>
       </c>
@@ -2570,7 +2608,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="71" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="84" t="s">
         <v>24</v>
       </c>
@@ -2583,7 +2621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="84" t="s">
         <v>43</v>
       </c>
@@ -2596,7 +2634,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:7" ht="31.2" x14ac:dyDescent="0.25">
       <c r="B73" s="56"/>
       <c r="C73" s="58"/>
       <c r="D73" s="61"/>
@@ -2609,15 +2647,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="31"/>
       <c r="C74" s="32"/>
       <c r="D74" s="32"/>
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
     </row>
-    <row r="75" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="87" t="s">
         <v>56</v>
       </c>
@@ -2630,7 +2668,7 @@
         <v>121.6</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="35" t="s">
         <v>65</v>
       </c>
@@ -2641,7 +2679,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="63">
         <v>20</v>
       </c>
@@ -2650,17 +2688,17 @@
         <v>28</v>
       </c>
       <c r="D80" s="63">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" s="81" t="s">
         <v>68</v>
       </c>
       <c r="C81" s="82"/>
       <c r="D81" s="83"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="59" t="s">
         <v>59</v>
       </c>
@@ -2674,10 +2712,10 @@
       </c>
       <c r="D82" s="63">
         <f>$G$76*D80</f>
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+        <v>486.4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="59" t="s">
         <v>63</v>
       </c>
@@ -2691,10 +2729,10 @@
       </c>
       <c r="D83" s="65">
         <f>D82/(8*5*4+2)</f>
-        <v>7.5061728395061724</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3.0024691358024689</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="60" t="s">
         <v>61</v>
       </c>
@@ -2708,7 +2746,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="60" t="s">
         <v>62</v>
       </c>
@@ -2722,10 +2760,10 @@
       </c>
       <c r="D85" s="65">
         <f>D83/D84</f>
-        <v>1.8765432098765431</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="31.5" x14ac:dyDescent="0.2">
+        <v>0.75061728395061722</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="31.2" x14ac:dyDescent="0.25">
       <c r="C88" s="67" t="s">
         <v>109</v>
       </c>
@@ -2736,7 +2774,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C89" s="25" t="s">
         <v>112</v>
       </c>
@@ -2745,10 +2783,10 @@
       </c>
       <c r="E89" s="69">
         <f>E90/2</f>
-        <v>304</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>121.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C90" s="25" t="s">
         <v>113</v>
       </c>
@@ -2757,10 +2795,10 @@
       </c>
       <c r="E90" s="69">
         <f>E91/2</f>
-        <v>608</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>243.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C91" s="25" t="s">
         <v>114</v>
       </c>
@@ -2769,10 +2807,10 @@
       </c>
       <c r="E91" s="70">
         <f>D82</f>
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>486.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C92" s="25" t="s">
         <v>115</v>
       </c>
@@ -2781,10 +2819,10 @@
       </c>
       <c r="E92" s="69">
         <f>(15*(SUM(E89:E91))/SUM(D89:D91))</f>
-        <v>456</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>182.39999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C93" s="25" t="s">
         <v>116</v>
       </c>
@@ -2793,10 +2831,10 @@
       </c>
       <c r="E93" s="69">
         <f>E92</f>
-        <v>456</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>182.39999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C94" s="25" t="s">
         <v>117</v>
       </c>
@@ -2805,55 +2843,55 @@
       </c>
       <c r="E94" s="69">
         <f>SUM(E89:E93)</f>
-        <v>3040</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="23"/>
       <c r="C96" s="75"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="76"/>
       <c r="C97" s="76"/>
       <c r="D97" s="35" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="77"/>
       <c r="C98" s="77"/>
       <c r="D98" s="63">
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="15"/>
       <c r="C99" s="78"/>
       <c r="D99" s="35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B100" s="77"/>
       <c r="C100" s="59" t="s">
         <v>59</v>
       </c>
       <c r="D100" s="72">
         <f>E94</f>
-        <v>3040</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="79"/>
       <c r="C101" s="59" t="s">
         <v>63</v>
       </c>
       <c r="D101" s="73">
         <f>D100/(8*5*4+2)</f>
-        <v>18.765432098765434</v>
-      </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+        <v>7.5061728395061724</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B102" s="80"/>
       <c r="C102" s="60" t="s">
         <v>61</v>
@@ -2862,17 +2900,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B103" s="79"/>
       <c r="C103" s="60" t="s">
         <v>62</v>
       </c>
       <c r="D103" s="73">
         <f>D101/D102</f>
-        <v>4.6913580246913584</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+        <v>1.8765432098765431</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="23"/>
       <c r="C104" s="75"/>
     </row>

</xml_diff>